<commit_message>
update specific reagent batch searches
</commit_message>
<xml_diff>
--- a/sampledata/sample_primary_cell_batch.xlsx
+++ b/sampledata/sample_primary_cell_batch.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="248">
   <si>
     <t>Facility ID</t>
   </si>
@@ -46,6 +46,9 @@
     <t>PC_Transient_Modification</t>
   </si>
   <si>
+    <t>PC_Source_Information</t>
+  </si>
+  <si>
     <t>PC_Culture_Conditions</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
     <t>transient modification 1</t>
   </si>
   <si>
+    <t>pc_source_information1</t>
+  </si>
+  <si>
     <t>culture condition 1</t>
   </si>
   <si>
@@ -118,6 +124,9 @@
     <t>transient modification 2</t>
   </si>
   <si>
+    <t>pc_source_information2</t>
+  </si>
+  <si>
     <t>culture condition 2</t>
   </si>
   <si>
@@ -142,6 +151,9 @@
     <t>transient modification 3</t>
   </si>
   <si>
+    <t>pc_source_information3</t>
+  </si>
+  <si>
     <t>culture condition 3</t>
   </si>
   <si>
@@ -166,6 +178,9 @@
     <t>transient modification 4</t>
   </si>
   <si>
+    <t>pc_source_information4</t>
+  </si>
+  <si>
     <t>culture condition 4</t>
   </si>
   <si>
@@ -190,6 +205,9 @@
     <t>transient modification 5</t>
   </si>
   <si>
+    <t>pc_source_information5</t>
+  </si>
+  <si>
     <t>culture condition 5</t>
   </si>
   <si>
@@ -211,6 +229,9 @@
     <t>transient modification 6</t>
   </si>
   <si>
+    <t>pc_source_information6</t>
+  </si>
+  <si>
     <t>culture condition 6</t>
   </si>
   <si>
@@ -235,6 +256,9 @@
     <t>transient modification 7</t>
   </si>
   <si>
+    <t>pc_source_information7</t>
+  </si>
+  <si>
     <t>culture condition 7</t>
   </si>
   <si>
@@ -250,6 +274,9 @@
     <t>transient modification 8</t>
   </si>
   <si>
+    <t>pc_source_information8</t>
+  </si>
+  <si>
     <t>culture condition 8</t>
   </si>
   <si>
@@ -271,6 +298,9 @@
     <t>transient modification 9</t>
   </si>
   <si>
+    <t>pc_source_information9</t>
+  </si>
+  <si>
     <t>culture condition 9</t>
   </si>
   <si>
@@ -292,6 +322,9 @@
     <t>transient modification 10</t>
   </si>
   <si>
+    <t>pc_source_information10</t>
+  </si>
+  <si>
     <t>culture condition 10</t>
   </si>
   <si>
@@ -310,6 +343,9 @@
     <t>transient modification 11</t>
   </si>
   <si>
+    <t>pc_source_information11</t>
+  </si>
+  <si>
     <t>culture condition 11</t>
   </si>
   <si>
@@ -328,6 +364,9 @@
     <t>transient modification 12</t>
   </si>
   <si>
+    <t>pc_source_information12</t>
+  </si>
+  <si>
     <t>culture condition 12</t>
   </si>
   <si>
@@ -346,6 +385,9 @@
     <t>transient modification 13</t>
   </si>
   <si>
+    <t>pc_source_information13</t>
+  </si>
+  <si>
     <t>culture condition 13</t>
   </si>
   <si>
@@ -364,6 +406,9 @@
     <t>transient modification 14</t>
   </si>
   <si>
+    <t>pc_source_information14</t>
+  </si>
+  <si>
     <t>culture condition 14</t>
   </si>
   <si>
@@ -382,6 +427,9 @@
     <t>transient modification 15</t>
   </si>
   <si>
+    <t>pc_source_information15</t>
+  </si>
+  <si>
     <t>culture condition 15</t>
   </si>
   <si>
@@ -400,6 +448,9 @@
     <t>transient modification 16</t>
   </si>
   <si>
+    <t>pc_source_information16</t>
+  </si>
+  <si>
     <t>culture condition 16</t>
   </si>
   <si>
@@ -418,6 +469,9 @@
     <t>transient modification 17</t>
   </si>
   <si>
+    <t>pc_source_information17</t>
+  </si>
+  <si>
     <t>culture condition 17</t>
   </si>
   <si>
@@ -439,6 +493,9 @@
     <t>transient modification 18</t>
   </si>
   <si>
+    <t>pc_source_information18</t>
+  </si>
+  <si>
     <t>culture condition 18</t>
   </si>
   <si>
@@ -457,6 +514,9 @@
     <t>transient modification 19</t>
   </si>
   <si>
+    <t>pc_source_information19</t>
+  </si>
+  <si>
     <t>culture condition 19</t>
   </si>
   <si>
@@ -472,6 +532,9 @@
     <t>transient modification 20</t>
   </si>
   <si>
+    <t>pc_source_information20</t>
+  </si>
+  <si>
     <t>culture condition 20</t>
   </si>
   <si>
@@ -487,6 +550,9 @@
     <t>transient modification 21</t>
   </si>
   <si>
+    <t>pc_source_information21</t>
+  </si>
+  <si>
     <t>culture condition 21</t>
   </si>
   <si>
@@ -505,6 +571,9 @@
     <t>transient modification 22</t>
   </si>
   <si>
+    <t>pc_source_information22</t>
+  </si>
+  <si>
     <t>culture condition 22</t>
   </si>
   <si>
@@ -523,6 +592,9 @@
     <t>transient modification 23</t>
   </si>
   <si>
+    <t>pc_source_information23</t>
+  </si>
+  <si>
     <t>culture condition 23</t>
   </si>
   <si>
@@ -541,6 +613,9 @@
     <t>transient modification 24</t>
   </si>
   <si>
+    <t>pc_source_information24</t>
+  </si>
+  <si>
     <t>culture condition 24</t>
   </si>
   <si>
@@ -559,6 +634,9 @@
     <t>transient modification 25</t>
   </si>
   <si>
+    <t>pc_source_information25</t>
+  </si>
+  <si>
     <t>culture condition 25</t>
   </si>
   <si>
@@ -577,6 +655,9 @@
     <t>transient modification 26</t>
   </si>
   <si>
+    <t>pc_source_information26</t>
+  </si>
+  <si>
     <t>culture condition 26</t>
   </si>
   <si>
@@ -595,6 +676,9 @@
     <t>transient modification 27</t>
   </si>
   <si>
+    <t>pc_source_information27</t>
+  </si>
+  <si>
     <t>culture condition 27</t>
   </si>
   <si>
@@ -613,6 +697,9 @@
     <t>transient modification 28</t>
   </si>
   <si>
+    <t>pc_source_information28</t>
+  </si>
+  <si>
     <t>culture condition 28</t>
   </si>
   <si>
@@ -631,6 +718,9 @@
     <t>transient modification 29</t>
   </si>
   <si>
+    <t>pc_source_information29</t>
+  </si>
+  <si>
     <t>culture condition 29</t>
   </si>
   <si>
@@ -649,6 +739,9 @@
     <t>transient modification 30</t>
   </si>
   <si>
+    <t>pc_source_information30</t>
+  </si>
+  <si>
     <t>culture condition 30</t>
   </si>
   <si>
@@ -665,6 +758,9 @@
   </si>
   <si>
     <t>transient modification 31</t>
+  </si>
+  <si>
+    <t>pc_source_information31</t>
   </si>
   <si>
     <t>culture condition 31</t>
@@ -799,10 +895,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -813,11 +909,11 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.5612244897959"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.9234693877551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="8" style="1" width="21.7857142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="25.0255102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.3163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="8" style="1" width="21.7857142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="25.0255102040816"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.3163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,10 +947,10 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
@@ -866,1445 +962,1541 @@
       <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0"/>
+      <c r="P1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>24</v>
+      <c r="L2" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="2"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>26</v>
+        <v>43</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="3" t="n">
+        <v>52</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="2"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>24</v>
+        <v>61</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="3" t="n">
+        <v>69</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7" s="5"/>
+      <c r="L7" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="3" t="n">
+        <v>78</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>42</v>
+      <c r="L8" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P8" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>87020501</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="5"/>
+      <c r="L9" s="4"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="2"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="L10" s="4"/>
       <c r="M10" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>24</v>
+      <c r="L11" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="J12" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K12" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>24</v>
+      <c r="L12" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P12" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J13" s="3" t="n">
+        <v>114</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>24</v>
+      <c r="L13" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J14" s="3" t="n">
+        <v>121</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>24</v>
+      <c r="L14" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P14" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J15" s="3" t="n">
+        <v>128</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K15" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="K15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>24</v>
+      <c r="L15" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P15" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J16" s="3" t="n">
+        <v>135</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K16" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>24</v>
+      <c r="L16" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P16" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="J17" s="3" t="n">
+        <v>142</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="K17" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>24</v>
+      <c r="L17" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P17" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="B18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="J18" s="3" t="n">
+        <v>149</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K18" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="L18" s="4"/>
       <c r="M18" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P18" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="B19" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J19" s="3" t="n">
+        <v>157</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="K19" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="L19" s="4"/>
       <c r="M19" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P19" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="B20" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J20" s="3" t="n">
+        <v>164</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K20" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="K20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>24</v>
+      <c r="L20" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P20" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="B21" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>99040201</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="J21" s="3" t="n">
+        <v>170</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K21" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>24</v>
+      <c r="L21" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P21" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="B22" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>98032302</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J22" s="3" t="n">
+        <v>176</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="K22" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="K22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>24</v>
+      <c r="L22" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P22" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="B23" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="J23" s="3" t="n">
+        <v>183</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K23" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="K23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>24</v>
+      <c r="L23" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P23" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="B24" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="J24" s="3" t="n">
+        <v>190</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="K24" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="K24" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>24</v>
+      <c r="L24" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P24" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="B25" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="J25" s="3" t="n">
+        <v>197</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K25" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="K25" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>24</v>
+      <c r="L25" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P25" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="B26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="J26" s="3" t="n">
+        <v>204</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="K26" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="K26" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>24</v>
+      <c r="L26" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P26" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="B27" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J27" s="3" t="n">
+        <v>211</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K27" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="K27" s="4"/>
-      <c r="L27" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="L27" s="4"/>
       <c r="M27" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P27" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="B28" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="J28" s="3" t="n">
+        <v>218</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="K28" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="K28" s="4"/>
-      <c r="L28" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="L28" s="4"/>
       <c r="M28" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P28" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="B29" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="J29" s="3" t="n">
+        <v>225</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="K29" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="K29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>24</v>
+      <c r="L29" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P29" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="B30" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="K30" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="J30" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P30" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="B31" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>208</v>
+        <v>238</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="J31" s="3" t="n">
+        <v>239</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="K31" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="K31" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>24</v>
+      <c r="L31" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P31" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>210</v>
+        <v>241</v>
       </c>
       <c r="B32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="J32" s="3" t="n">
+        <v>246</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="K32" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="K32" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>24</v>
+      <c r="L32" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P32" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q32" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2622,248 +2814,248 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial differentiated cell implementation
</commit_message>
<xml_diff>
--- a/sampledata/sample_primary_cell_batch.xlsx
+++ b/sampledata/sample_primary_cell_batch.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,11 +16,16 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Sheet_Title" vbProcedure="false">"Sheet1"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="220">
   <si>
     <t>Facility ID</t>
   </si>
@@ -91,7 +96,7 @@
     <t>2014-02-05</t>
   </si>
   <si>
-    <t>quality verification 1</t>
+    <t>PASS</t>
   </si>
   <si>
     <t>culture condition 1</t>
@@ -124,7 +129,7 @@
     <t>2014-04</t>
   </si>
   <si>
-    <t>quality verification 1-2</t>
+    <t>FAIL</t>
   </si>
   <si>
     <t>culture condition 2</t>
@@ -151,9 +156,6 @@
     <t>2013</t>
   </si>
   <si>
-    <t>quality verification 2</t>
-  </si>
-  <si>
     <t>culture condition 3</t>
   </si>
   <si>
@@ -178,9 +180,6 @@
     <t>2016-02-02</t>
   </si>
   <si>
-    <t>quality verification 2-2</t>
-  </si>
-  <si>
     <t>culture condition 4</t>
   </si>
   <si>
@@ -205,9 +204,6 @@
     <t>2015-11-11</t>
   </si>
   <si>
-    <t>quality verification 3</t>
-  </si>
-  <si>
     <t>culture condition 5</t>
   </si>
   <si>
@@ -229,9 +225,6 @@
     <t>2015-11</t>
   </si>
   <si>
-    <t>quality verification 4</t>
-  </si>
-  <si>
     <t>culture condition 6</t>
   </si>
   <si>
@@ -256,9 +249,6 @@
     <t>2015</t>
   </si>
   <si>
-    <t>quality verification 5</t>
-  </si>
-  <si>
     <t>culture condition 7</t>
   </si>
   <si>
@@ -271,9 +261,6 @@
     <t>pc_source_information8</t>
   </si>
   <si>
-    <t>quality verification 6</t>
-  </si>
-  <si>
     <t>culture condition 8</t>
   </si>
   <si>
@@ -295,9 +282,6 @@
     <t>pc_source_information9</t>
   </si>
   <si>
-    <t>quality verification 7</t>
-  </si>
-  <si>
     <t>culture condition 9</t>
   </si>
   <si>
@@ -319,9 +303,6 @@
     <t>pc_source_information10</t>
   </si>
   <si>
-    <t>quality verification 8</t>
-  </si>
-  <si>
     <t>culture condition 10</t>
   </si>
   <si>
@@ -340,9 +321,6 @@
     <t>pc_source_information11</t>
   </si>
   <si>
-    <t>quality verification 9</t>
-  </si>
-  <si>
     <t>culture condition 11</t>
   </si>
   <si>
@@ -361,9 +339,6 @@
     <t>pc_source_information12</t>
   </si>
   <si>
-    <t>quality verification 10</t>
-  </si>
-  <si>
     <t>culture condition 12</t>
   </si>
   <si>
@@ -382,9 +357,6 @@
     <t>pc_source_information13</t>
   </si>
   <si>
-    <t>quality verification 11</t>
-  </si>
-  <si>
     <t>culture condition 13</t>
   </si>
   <si>
@@ -403,9 +375,6 @@
     <t>pc_source_information14</t>
   </si>
   <si>
-    <t>quality verification 12</t>
-  </si>
-  <si>
     <t>culture condition 14</t>
   </si>
   <si>
@@ -424,9 +393,6 @@
     <t>pc_source_information15</t>
   </si>
   <si>
-    <t>quality verification 13</t>
-  </si>
-  <si>
     <t>culture condition 15</t>
   </si>
   <si>
@@ -445,9 +411,6 @@
     <t>pc_source_information16</t>
   </si>
   <si>
-    <t>quality verification 14</t>
-  </si>
-  <si>
     <t>culture condition 16</t>
   </si>
   <si>
@@ -466,9 +429,6 @@
     <t>pc_source_information17</t>
   </si>
   <si>
-    <t>quality verification 15</t>
-  </si>
-  <si>
     <t>culture condition 17</t>
   </si>
   <si>
@@ -490,9 +450,6 @@
     <t>pc_source_information18</t>
   </si>
   <si>
-    <t>quality verification 16</t>
-  </si>
-  <si>
     <t>culture condition 18</t>
   </si>
   <si>
@@ -511,9 +468,6 @@
     <t>pc_source_information19</t>
   </si>
   <si>
-    <t>quality verification 17</t>
-  </si>
-  <si>
     <t>culture condition 19</t>
   </si>
   <si>
@@ -529,9 +483,6 @@
     <t>pc_source_information20</t>
   </si>
   <si>
-    <t>quality verification 18</t>
-  </si>
-  <si>
     <t>culture condition 20</t>
   </si>
   <si>
@@ -547,9 +498,6 @@
     <t>pc_source_information21</t>
   </si>
   <si>
-    <t>quality verification 19</t>
-  </si>
-  <si>
     <t>culture condition 21</t>
   </si>
   <si>
@@ -568,9 +516,6 @@
     <t>pc_source_information22</t>
   </si>
   <si>
-    <t>quality verification 20</t>
-  </si>
-  <si>
     <t>culture condition 22</t>
   </si>
   <si>
@@ -589,9 +534,6 @@
     <t>pc_source_information23</t>
   </si>
   <si>
-    <t>quality verification 21</t>
-  </si>
-  <si>
     <t>culture condition 23</t>
   </si>
   <si>
@@ -610,9 +552,6 @@
     <t>pc_source_information24</t>
   </si>
   <si>
-    <t>quality verification 22</t>
-  </si>
-  <si>
     <t>culture condition 24</t>
   </si>
   <si>
@@ -631,9 +570,6 @@
     <t>pc_source_information25</t>
   </si>
   <si>
-    <t>quality verification 23</t>
-  </si>
-  <si>
     <t>culture condition 25</t>
   </si>
   <si>
@@ -652,9 +588,6 @@
     <t>pc_source_information26</t>
   </si>
   <si>
-    <t>quality verification 24</t>
-  </si>
-  <si>
     <t>culture condition 26</t>
   </si>
   <si>
@@ -673,9 +606,6 @@
     <t>pc_source_information27</t>
   </si>
   <si>
-    <t>quality verification 25</t>
-  </si>
-  <si>
     <t>culture condition 27</t>
   </si>
   <si>
@@ -694,9 +624,6 @@
     <t>pc_source_information28</t>
   </si>
   <si>
-    <t>quality verification 26</t>
-  </si>
-  <si>
     <t>culture condition 28</t>
   </si>
   <si>
@@ -715,9 +642,6 @@
     <t>pc_source_information29</t>
   </si>
   <si>
-    <t>quality verification 27</t>
-  </si>
-  <si>
     <t>culture condition 29</t>
   </si>
   <si>
@@ -736,9 +660,6 @@
     <t>pc_source_information30</t>
   </si>
   <si>
-    <t>quality verification 28</t>
-  </si>
-  <si>
     <t>culture condition 30</t>
   </si>
   <si>
@@ -755,9 +676,6 @@
   </si>
   <si>
     <t>pc_source_information31</t>
-  </si>
-  <si>
-    <t>quality verification 29</t>
   </si>
   <si>
     <t>culture condition 31</t>
@@ -937,27 +855,27 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.9234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="21.7857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="21.7857142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="25.0255102040816"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.3163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,16 +1060,16 @@
         <v>42</v>
       </c>
       <c r="I5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="K5" s="9" t="n">
         <v>1</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M5" s="12" t="s">
         <v>28</v>
@@ -1163,7 +1081,7 @@
         <v>28</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,34 +1092,34 @@
         <v>2</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="K6" s="9" t="n">
         <v>3</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
@@ -1210,40 +1128,40 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="H7" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="I7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="K7" s="9" t="n">
         <v>1</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M7" s="12" t="s">
         <v>26</v>
@@ -1260,40 +1178,40 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="9" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="I8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="K8" s="9" t="n">
         <v>4</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
@@ -1302,57 +1220,57 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="K9" s="9" t="n">
         <v>3</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B10" s="9" t="n">
         <v>2</v>
@@ -1365,23 +1283,23 @@
         <v>87020501</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="9" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K10" s="9" t="n">
         <v>2</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
@@ -1390,38 +1308,38 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B11" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="9" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K11" s="9" t="n">
         <v>4</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>26</v>
@@ -1438,40 +1356,40 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B12" s="9" t="n">
         <v>2</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="K12" s="9" t="n">
         <v>2</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="M12" s="12" t="s">
         <v>26</v>
@@ -1483,45 +1401,45 @@
         <v>27</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B13" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>33</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>106</v>
+        <v>23</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="K13" s="9" t="n">
         <v>5</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="M13" s="12" t="s">
         <v>26</v>
@@ -1533,45 +1451,45 @@
         <v>27</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B14" s="9" t="n">
         <v>2</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>42</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>113</v>
+        <v>34</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="K14" s="9" t="n">
         <v>4</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="M14" s="12" t="s">
         <v>26</v>
@@ -1588,40 +1506,40 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B15" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>120</v>
+        <v>23</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="K15" s="9" t="n">
         <v>3</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="M15" s="12" t="s">
         <v>26</v>
@@ -1633,45 +1551,45 @@
         <v>27</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="K16" s="9" t="n">
         <v>5</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="M16" s="12" t="s">
         <v>26</v>
@@ -1683,45 +1601,45 @@
         <v>27</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B17" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>20</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>134</v>
+        <v>34</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="K17" s="9" t="n">
         <v>3</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="M17" s="12" t="s">
         <v>26</v>
@@ -1733,45 +1651,45 @@
         <v>27</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>141</v>
+        <v>23</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="K18" s="9" t="n">
         <v>6</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="M18" s="12" t="s">
         <v>26</v>
@@ -1783,43 +1701,43 @@
         <v>27</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B19" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="9" t="s">
-        <v>148</v>
+        <v>34</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="K19" s="9" t="n">
         <v>5</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="M19" s="12" t="s">
         <v>26</v>
@@ -1831,43 +1749,43 @@
         <v>27</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B20" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="9" t="s">
-        <v>156</v>
+        <v>23</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="K20" s="9" t="n">
         <v>4</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="M20" s="12" t="s">
         <v>26</v>
@@ -1879,45 +1797,45 @@
         <v>27</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="B21" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>163</v>
+        <v>34</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="K21" s="9" t="n">
         <v>6</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="M21" s="12" t="s">
         <v>26</v>
@@ -1929,18 +1847,18 @@
         <v>27</v>
       </c>
       <c r="P21" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B22" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>30</v>
@@ -1949,25 +1867,25 @@
         <v>99040201</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>33</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="K22" s="9" t="n">
         <v>4</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="M22" s="12" t="s">
         <v>26</v>
@@ -1979,18 +1897,18 @@
         <v>27</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B23" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>30</v>
@@ -2002,22 +1920,22 @@
         <v>20</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>42</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>175</v>
+        <v>34</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="K23" s="9" t="n">
         <v>7</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="M23" s="12" t="s">
         <v>26</v>
@@ -2029,45 +1947,45 @@
         <v>27</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>182</v>
+        <v>23</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="K24" s="9" t="n">
         <v>6</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="M24" s="12" t="s">
         <v>26</v>
@@ -2079,45 +1997,45 @@
         <v>27</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="B25" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="F25" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>60</v>
-      </c>
       <c r="I25" s="9" t="s">
-        <v>189</v>
+        <v>34</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="K25" s="9" t="n">
         <v>5</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="M25" s="12" t="s">
         <v>26</v>
@@ -2129,45 +2047,45 @@
         <v>27</v>
       </c>
       <c r="P25" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B26" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>196</v>
+        <v>23</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="K26" s="9" t="n">
         <v>7</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="M26" s="12" t="s">
         <v>26</v>
@@ -2179,45 +2097,45 @@
         <v>27</v>
       </c>
       <c r="P26" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="B27" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>203</v>
+        <v>34</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="K27" s="9" t="n">
         <v>5</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="M27" s="12" t="s">
         <v>26</v>
@@ -2229,43 +2147,43 @@
         <v>27</v>
       </c>
       <c r="P27" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="B28" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="9" t="s">
-        <v>210</v>
+        <v>23</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="K28" s="9" t="n">
         <v>8</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="M28" s="12" t="s">
         <v>26</v>
@@ -2277,43 +2195,43 @@
         <v>27</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="B29" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="9" t="s">
-        <v>217</v>
+        <v>23</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="K29" s="9" t="n">
         <v>7</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="M29" s="12" t="s">
         <v>26</v>
@@ -2325,45 +2243,45 @@
         <v>27</v>
       </c>
       <c r="P29" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="B30" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>224</v>
+        <v>34</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="K30" s="9" t="n">
         <v>6</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="M30" s="12" t="s">
         <v>26</v>
@@ -2375,45 +2293,45 @@
         <v>27</v>
       </c>
       <c r="P30" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
       <c r="B31" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>228</v>
+        <v>202</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>33</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>231</v>
+        <v>23</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="K31" s="9" t="n">
         <v>8</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="M31" s="12" t="s">
         <v>26</v>
@@ -2425,45 +2343,45 @@
         <v>27</v>
       </c>
       <c r="P31" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
-        <v>234</v>
+        <v>207</v>
       </c>
       <c r="B32" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>236</v>
+        <v>209</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>42</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>238</v>
+        <v>34</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="K32" s="9" t="n">
         <v>6</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="M32" s="12" t="s">
         <v>26</v>
@@ -2475,45 +2393,45 @@
         <v>27</v>
       </c>
       <c r="P32" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="B33" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>245</v>
+        <v>23</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="K33" s="9" t="n">
         <v>9</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="M33" s="12" t="s">
         <v>26</v>
@@ -2525,7 +2443,7 @@
         <v>27</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2552,7 +2470,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="8" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="8" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,43 +2516,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>